<commit_message>
added length of sprints to scrum spreadsheet
</commit_message>
<xml_diff>
--- a/Nonreact/Scrum.xlsx
+++ b/Nonreact/Scrum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iMakeBabbies/coding_mac/repositories/grocery_inventory_app/Nonreact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD2946B-CAB9-234F-910A-2B08D9D98FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33AB6DD-3ADF-9E48-9240-DE896CC2B137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5240" yWindow="5240" windowWidth="28040" windowHeight="17440" xr2:uid="{E169FF0C-8F15-8A49-9044-0CD5B695CC1A}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t>Code inventory view page using a table</t>
   </si>
   <si>
-    <t>Sprint Backlog #1</t>
-  </si>
-  <si>
     <t>Code login page</t>
   </si>
   <si>
@@ -102,7 +99,10 @@
     <t>Remind user of old inventory</t>
   </si>
   <si>
-    <t>Sprint Backlog #2</t>
+    <t>Sprint Backlog #1 - 2 Weeks</t>
+  </si>
+  <si>
+    <t>Sprint Backlog #2 - 2 Weeks</t>
   </si>
 </sst>
 </file>
@@ -635,7 +635,7 @@
   <dimension ref="B3:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,7 +655,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="9"/>
       <c r="G4" s="15" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
@@ -815,7 +815,7 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="G12" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H12" s="11">
         <v>3</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="G13" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10">
@@ -839,7 +839,7 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="G14" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -853,7 +853,7 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="G15" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>

</xml_diff>

<commit_message>
updated Scrum with test cases
</commit_message>
<xml_diff>
--- a/Nonreact/Scrum.xlsx
+++ b/Nonreact/Scrum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iMakeBabbies/coding_mac/repositories/grocery_inventory_app/Nonreact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33AB6DD-3ADF-9E48-9240-DE896CC2B137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951BF623-C0A8-2B40-9470-8103E681FFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5240" yWindow="5240" windowWidth="28040" windowHeight="17440" xr2:uid="{E169FF0C-8F15-8A49-9044-0CD5B695CC1A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{E169FF0C-8F15-8A49-9044-0CD5B695CC1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Requirements</t>
   </si>
@@ -103,6 +103,36 @@
   </si>
   <si>
     <t>Sprint Backlog #2 - 2 Weeks</t>
+  </si>
+  <si>
+    <t>Test Cases</t>
+  </si>
+  <si>
+    <t>User must be able to register new products to the inventory</t>
+  </si>
+  <si>
+    <t>User must be able to view inventory</t>
+  </si>
+  <si>
+    <t>User must be able to delete items from inventory</t>
+  </si>
+  <si>
+    <t>User must be able to sign up</t>
+  </si>
+  <si>
+    <t>User must be able to login</t>
+  </si>
+  <si>
+    <t>Test case 1</t>
+  </si>
+  <si>
+    <t>Test case 2</t>
+  </si>
+  <si>
+    <t>Test case 3</t>
+  </si>
+  <si>
+    <t>Test case 4</t>
   </si>
 </sst>
 </file>
@@ -220,15 +250,22 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -241,9 +278,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -256,17 +291,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -282,18 +306,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -304,25 +331,317 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -333,6 +652,36 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DF6AA103-22A9-2F4E-B6D3-F92ED58317A3}" name="Table1" displayName="Table1" ref="G5:L11" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="15" tableBorderDxfId="16">
+  <autoFilter ref="G5:L11" xr:uid="{DF6AA103-22A9-2F4E-B6D3-F92ED58317A3}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{BFFBA90E-F0D7-9344-B2F0-87379870C651}" name="Task" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{0B322583-F91F-7E4D-81E7-A9C2CF0693D5}" name="Mon" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{74245554-6B6D-264E-A37D-4C114EC306B3}" name="Tues" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{D6FCFFF8-651D-E84B-9901-97FD4FC62F27}" name="Wed" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{B4B4FB33-9845-9942-B0E7-37905140C946}" name="Thur" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{3DC8E9AB-3816-C744-B5EA-9AD89F787634}" name="Fri" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6ABC9B9D-6456-7241-ACDD-46F7533B969E}" name="Table2" displayName="Table2" ref="G14:L20" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7">
+  <autoFilter ref="G14:L20" xr:uid="{6ABC9B9D-6456-7241-ACDD-46F7533B969E}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{AA808488-8AE1-E341-B66B-8CD0DC0D22CB}" name="Task"/>
+    <tableColumn id="2" xr3:uid="{7D09E7B4-F666-5649-962F-716BA57582C6}" name="Mon" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{8B63D63E-FEF3-9B45-A636-0F1537464D37}" name="Tues" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{985715A8-8EEF-694C-8CEC-F574217EDFD3}" name="Wed" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{E723B9D7-B67F-724D-AF8A-821E63274759}" name="Thur" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{51AEB49C-E936-1C4B-A9CB-67F0E96AB161}" name="Fri" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -632,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE6C85DD-DBE8-A949-880E-C4B03D3FC2B8}">
-  <dimension ref="B3:L15"/>
+  <dimension ref="B3:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -648,46 +997,46 @@
   <sheetData>
     <row r="3" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="G4" s="15" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+      <c r="G4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
     </row>
     <row r="5" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="G5" s="12" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="G5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="L5" s="17" t="s">
         <v>11</v>
       </c>
     </row>
@@ -695,182 +1044,304 @@
       <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="G6" s="11" t="s">
+      <c r="C6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="G6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="11">
-        <v>2</v>
-      </c>
-      <c r="I6" s="11">
-        <v>2</v>
-      </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="H6" s="5">
+        <v>2</v>
+      </c>
+      <c r="I6" s="5">
+        <v>2</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="10" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="G7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="10">
-        <v>2</v>
-      </c>
-      <c r="I7" s="10">
-        <v>2</v>
-      </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
+      <c r="H7" s="4">
+        <v>2</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="10" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="G8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="G9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10">
-        <v>2</v>
-      </c>
-      <c r="K8" s="10">
-        <v>2</v>
-      </c>
-      <c r="L8" s="10"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="4">
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4">
+        <v>2</v>
+      </c>
+      <c r="K9" s="4">
+        <v>2</v>
+      </c>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B10" s="2">
+        <v>6</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="G10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4">
+        <v>2</v>
+      </c>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="2">
+        <v>7</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="G11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4">
+        <v>2</v>
+      </c>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="13" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+      <c r="G14" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="G15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="5">
+        <v>3</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="G16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4">
+        <v>3</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B17" s="1">
+        <v>3</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="G17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4">
+        <v>2</v>
+      </c>
+      <c r="K17" s="4">
+        <v>2</v>
+      </c>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B18" s="1">
+        <v>4</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="G18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4">
+        <v>2</v>
+      </c>
+      <c r="L18" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B19" s="2">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="4">
-        <v>6</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="G10" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-    </row>
-    <row r="11" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="4">
-        <v>7</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="G11" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G12" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="11">
-        <v>3</v>
-      </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G13" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10">
-        <v>3</v>
-      </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G14" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10">
-        <v>2</v>
-      </c>
-      <c r="K14" s="10">
-        <v>2</v>
-      </c>
-      <c r="L14" s="10"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G15" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10">
-        <v>2</v>
-      </c>
-      <c r="L15" s="10">
-        <v>2</v>
-      </c>
+      <c r="C19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="G19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4">
+        <v>2</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B20" s="2"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="G20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4">
+        <v>2</v>
+      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B21" s="2"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="18">
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="G4:L4"/>
-    <mergeCell ref="G10:L10"/>
+    <mergeCell ref="G13:L13"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="C6:E6"/>
@@ -879,5 +1350,9 @@
     <mergeCell ref="C9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated with COCOMO equation
</commit_message>
<xml_diff>
--- a/Nonreact/Scrum.xlsx
+++ b/Nonreact/Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iMakeBabbies/coding_mac/repositories/grocery_inventory_app/Nonreact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951BF623-C0A8-2B40-9470-8103E681FFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D8722F-DD89-9049-BAFE-0149CDE169A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{E169FF0C-8F15-8A49-9044-0CD5B695CC1A}"/>
+    <workbookView xWindow="0" yWindow="11560" windowWidth="34560" windowHeight="10780" xr2:uid="{E169FF0C-8F15-8A49-9044-0CD5B695CC1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>Requirements</t>
   </si>
@@ -133,6 +133,66 @@
   </si>
   <si>
     <t>Test case 4</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>KLOC</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>E=a(KLOC)^b</t>
+  </si>
+  <si>
+    <t>.25^1.05</t>
+  </si>
+  <si>
+    <t>.23326 * 2.4</t>
+  </si>
+  <si>
+    <t>Effort</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>DevTime</t>
+  </si>
+  <si>
+    <t>SS=E/D</t>
+  </si>
+  <si>
+    <t>StaffSize</t>
+  </si>
+  <si>
+    <t>Persons</t>
+  </si>
+  <si>
+    <t>Months</t>
+  </si>
+  <si>
+    <t>P=KLOC/E</t>
+  </si>
+  <si>
+    <t>Prod</t>
+  </si>
+  <si>
+    <t>D=c*E^d</t>
+  </si>
+  <si>
+    <t>E^d = 0.802</t>
+  </si>
+  <si>
+    <t>KLOC/Person</t>
   </si>
 </sst>
 </file>
@@ -315,13 +375,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -337,50 +396,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -473,16 +499,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -629,16 +655,50 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -654,31 +714,145 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>386862</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>192943</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{732DBB78-78AD-1640-919F-9B991D6520A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13322300" y="635000"/>
+          <a:ext cx="3892062" cy="1424843"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>BASIC</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Effort(E) = ab * (KLOC)^bb(in Person-months)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>	</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>DevelopmentTime(D) = cb * (E)^db (in month)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Average staff size(SS) = E/D (in Person)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Productivity(P) = KLOC / E (in KLOC/Person-month)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DF6AA103-22A9-2F4E-B6D3-F92ED58317A3}" name="Table1" displayName="Table1" ref="G5:L11" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="15" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DF6AA103-22A9-2F4E-B6D3-F92ED58317A3}" name="Table1" displayName="Table1" ref="G5:L11" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14">
   <autoFilter ref="G5:L11" xr:uid="{DF6AA103-22A9-2F4E-B6D3-F92ED58317A3}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{BFFBA90E-F0D7-9344-B2F0-87379870C651}" name="Task" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{0B322583-F91F-7E4D-81E7-A9C2CF0693D5}" name="Mon" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{74245554-6B6D-264E-A37D-4C114EC306B3}" name="Tues" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{D6FCFFF8-651D-E84B-9901-97FD4FC62F27}" name="Wed" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{B4B4FB33-9845-9942-B0E7-37905140C946}" name="Thur" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{3DC8E9AB-3816-C744-B5EA-9AD89F787634}" name="Fri" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{BFFBA90E-F0D7-9344-B2F0-87379870C651}" name="Task" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{0B322583-F91F-7E4D-81E7-A9C2CF0693D5}" name="Mon" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{74245554-6B6D-264E-A37D-4C114EC306B3}" name="Tues" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{D6FCFFF8-651D-E84B-9901-97FD4FC62F27}" name="Wed" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{B4B4FB33-9845-9942-B0E7-37905140C946}" name="Thur" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{3DC8E9AB-3816-C744-B5EA-9AD89F787634}" name="Fri" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6ABC9B9D-6456-7241-ACDD-46F7533B969E}" name="Table2" displayName="Table2" ref="G14:L20" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6ABC9B9D-6456-7241-ACDD-46F7533B969E}" name="Table2" displayName="Table2" ref="G14:L20" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="G14:L20" xr:uid="{6ABC9B9D-6456-7241-ACDD-46F7533B969E}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{AA808488-8AE1-E341-B66B-8CD0DC0D22CB}" name="Task"/>
-    <tableColumn id="2" xr3:uid="{7D09E7B4-F666-5649-962F-716BA57582C6}" name="Mon" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{8B63D63E-FEF3-9B45-A636-0F1537464D37}" name="Tues" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{985715A8-8EEF-694C-8CEC-F574217EDFD3}" name="Wed" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{E723B9D7-B67F-724D-AF8A-821E63274759}" name="Thur" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{51AEB49C-E936-1C4B-A9CB-67F0E96AB161}" name="Fri" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{7D09E7B4-F666-5649-962F-716BA57582C6}" name="Mon" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{8B63D63E-FEF3-9B45-A636-0F1537464D37}" name="Tues" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{985715A8-8EEF-694C-8CEC-F574217EDFD3}" name="Wed" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{E723B9D7-B67F-724D-AF8A-821E63274759}" name="Thur" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{51AEB49C-E936-1C4B-A9CB-67F0E96AB161}" name="Fri" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -981,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE6C85DD-DBE8-A949-880E-C4B03D3FC2B8}">
-  <dimension ref="B3:L21"/>
+  <dimension ref="B3:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -995,60 +1169,96 @@
     <col min="7" max="7" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+    <row r="3" spans="2:28" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="G4" s="8" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+      <c r="G4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="U4" t="s">
+        <v>33</v>
+      </c>
+      <c r="V4">
+        <v>2.4</v>
+      </c>
+      <c r="X4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA4">
+        <v>0.55982240000000005</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="5" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="G5" s="15" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="G5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="9" t="s">
         <v>11</v>
       </c>
+      <c r="U5" t="s">
+        <v>34</v>
+      </c>
+      <c r="V5">
+        <v>0.25</v>
+      </c>
+      <c r="X5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA5">
+        <v>2.0059999999999998</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
       <c r="G6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1061,16 +1271,34 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
+      <c r="U6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V6">
+        <v>1.05</v>
+      </c>
+      <c r="X6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA6">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
       <c r="G7" s="4" t="s">
         <v>12</v>
       </c>
@@ -1083,16 +1311,34 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
+      <c r="U7" t="s">
+        <v>41</v>
+      </c>
+      <c r="V7">
+        <v>0.38</v>
+      </c>
+      <c r="X7" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA7">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>4</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
       <c r="G8" s="4" t="s">
         <v>29</v>
       </c>
@@ -1103,16 +1349,22 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
+      <c r="U8" t="s">
+        <v>42</v>
+      </c>
+      <c r="V8">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>5</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
       <c r="G9" s="4" t="s">
         <v>16</v>
       </c>
@@ -1126,15 +1378,15 @@
       </c>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>6</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
       <c r="G10" s="6" t="s">
         <v>30</v>
       </c>
@@ -1145,16 +1397,25 @@
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
+      <c r="U10" t="s">
+        <v>37</v>
+      </c>
+      <c r="V10">
+        <v>0.23326</v>
+      </c>
+      <c r="X10" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>7</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
       <c r="G11" s="6" t="s">
         <v>31</v>
       </c>
@@ -1165,52 +1426,58 @@
         <v>2</v>
       </c>
       <c r="L11" s="4"/>
+      <c r="U11" t="s">
+        <v>38</v>
+      </c>
+      <c r="V11">
+        <v>0.55982240000000005</v>
+      </c>
     </row>
-    <row r="13" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G13" s="9" t="s">
+    <row r="13" spans="2:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
     </row>
-    <row r="14" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+    <row r="14" spans="2:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="G14" s="15" t="s">
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="G14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="I14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J14" s="16" t="s">
+      <c r="J14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K14" s="16" t="s">
+      <c r="K14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L14" s="17" t="s">
+      <c r="L14" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <v>1</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
       <c r="G15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1222,15 +1489,15 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>2</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
       <c r="G16" s="4" t="s">
         <v>18</v>
       </c>
@@ -1246,11 +1513,11 @@
       <c r="B17" s="1">
         <v>3</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
       <c r="G17" s="4" t="s">
         <v>19</v>
       </c>
@@ -1268,11 +1535,11 @@
       <c r="B18" s="1">
         <v>4</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
       <c r="G18" s="6" t="s">
         <v>20</v>
       </c>
@@ -1290,11 +1557,11 @@
       <c r="B19" s="2">
         <v>5</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
       <c r="G19" s="6" t="s">
         <v>29</v>
       </c>
@@ -1308,9 +1575,9 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
       <c r="G20" s="6" t="s">
         <v>32</v>
       </c>
@@ -1324,20 +1591,12 @@
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="G4:L4"/>
@@ -1348,11 +1607,20 @@
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated Scrum spreadsheet with intermediate COCOMO
</commit_message>
<xml_diff>
--- a/Nonreact/Scrum.xlsx
+++ b/Nonreact/Scrum.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iMakeBabbies/coding_mac/repositories/grocery_inventory_app/Nonreact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D8722F-DD89-9049-BAFE-0149CDE169A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25C6DAB-FDC9-F543-AB85-BDF51865B414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="11560" windowWidth="34560" windowHeight="10780" xr2:uid="{E169FF0C-8F15-8A49-9044-0CD5B695CC1A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{E169FF0C-8F15-8A49-9044-0CD5B695CC1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="80">
   <si>
     <t>Requirements</t>
   </si>
@@ -193,13 +193,94 @@
   </si>
   <si>
     <t>KLOC/Person</t>
+  </si>
+  <si>
+    <t>Required Software Reliability</t>
+  </si>
+  <si>
+    <t>Size of Application Database</t>
+  </si>
+  <si>
+    <t>Complexity of The Product</t>
+  </si>
+  <si>
+    <t>Hardware Attributes</t>
+  </si>
+  <si>
+    <t>Runtime Performance Constraints</t>
+  </si>
+  <si>
+    <t>Volatility of the virtual machine environment</t>
+  </si>
+  <si>
+    <t>Required turnabout time</t>
+  </si>
+  <si>
+    <t>Analyst capability</t>
+  </si>
+  <si>
+    <t>Applications experience</t>
+  </si>
+  <si>
+    <t>Software engineer capability</t>
+  </si>
+  <si>
+    <t>Virtual machine experience</t>
+  </si>
+  <si>
+    <t>Programming language experience</t>
+  </si>
+  <si>
+    <t>Project Attributes</t>
+  </si>
+  <si>
+    <t>Application of software engineering methods</t>
+  </si>
+  <si>
+    <t>Use of software tools</t>
+  </si>
+  <si>
+    <t>Required development schedule</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Nominal</t>
+  </si>
+  <si>
+    <t>Product Attributes</t>
+  </si>
+  <si>
+    <t>Memory Contraints</t>
+  </si>
+  <si>
+    <t>Personnel Attributes</t>
+  </si>
+  <si>
+    <t>Very Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Effort Adjustment Factor</t>
+  </si>
+  <si>
+    <t>Cost Drivers</t>
+  </si>
+  <si>
+    <t>EAF</t>
+  </si>
+  <si>
+    <t>Intermediate Effort</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -215,8 +296,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +323,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -358,10 +451,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -381,6 +475,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -396,14 +496,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
@@ -816,6 +913,109 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>Productivity(P) = KLOC / E (in KLOC/Person-month)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>622301</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>444501</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD5CF6F3-ABB2-3549-B0B7-383429C9AED0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13322301" y="3378200"/>
+          <a:ext cx="3949700" cy="1390650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INTERMEDIATE</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Multiply all 15 Cost Drivers to get Effort Adjustment Factor(EAF)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>E(Effort) = ab(KLOC)bb * EAF(in Person-Month)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>D(Development Time) = cb(E)db (in month)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>SS (Avg Staff Size) = E/D (in persons)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>P (Productivity) = KLOC/E (in KLOC/Person-month)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1155,10 +1355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE6C85DD-DBE8-A949-880E-C4B03D3FC2B8}">
-  <dimension ref="B3:AB21"/>
+  <dimension ref="B3:AB45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AB8" sqref="AB8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1166,25 +1366,26 @@
     <col min="2" max="2" width="6.6640625" customWidth="1"/>
     <col min="5" max="5" width="20.5" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" customWidth="1"/>
-    <col min="7" max="7" width="32.6640625" customWidth="1"/>
+    <col min="7" max="7" width="38.33203125" customWidth="1"/>
+    <col min="26" max="26" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:28" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="G4" s="16" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15"/>
+      <c r="G4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
       <c r="U4" t="s">
         <v>33</v>
       </c>
@@ -1208,11 +1409,11 @@
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
       <c r="G5" s="7" t="s">
         <v>6</v>
       </c>
@@ -1254,11 +1455,11 @@
       <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
       <c r="G6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1377,6 +1578,19 @@
         <v>2</v>
       </c>
       <c r="L9" s="4"/>
+      <c r="U9" t="s">
+        <v>78</v>
+      </c>
+      <c r="V9">
+        <v>2.13</v>
+      </c>
+      <c r="Z9" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA9" s="19">
+        <f>AA4*V9</f>
+        <v>1.192421712</v>
+      </c>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
@@ -1397,15 +1611,6 @@
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="U10" t="s">
-        <v>37</v>
-      </c>
-      <c r="V10">
-        <v>0.23326</v>
-      </c>
-      <c r="X10" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
@@ -1427,29 +1632,40 @@
       </c>
       <c r="L11" s="4"/>
       <c r="U11" t="s">
+        <v>37</v>
+      </c>
+      <c r="V11">
+        <v>0.23326</v>
+      </c>
+      <c r="X11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="U12" t="s">
         <v>38</v>
       </c>
-      <c r="V11">
+      <c r="V12">
         <v>0.55982240000000005</v>
       </c>
     </row>
     <row r="13" spans="2:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
     </row>
     <row r="14" spans="2:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="15"/>
       <c r="G14" s="7" t="s">
         <v>6</v>
       </c>
@@ -1473,11 +1689,11 @@
       <c r="B15" s="3">
         <v>1</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
       <c r="G15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1493,11 +1709,11 @@
       <c r="B16" s="1">
         <v>2</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
       <c r="G16" s="4" t="s">
         <v>18</v>
       </c>
@@ -1595,8 +1811,218 @@
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
     </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G24" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G25" s="18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" t="s">
+        <v>69</v>
+      </c>
+      <c r="I26">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I27">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" t="s">
+        <v>70</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G29" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>57</v>
+      </c>
+      <c r="H30" t="s">
+        <v>70</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" t="s">
+        <v>70</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>58</v>
+      </c>
+      <c r="H32" t="s">
+        <v>69</v>
+      </c>
+      <c r="I32">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>59</v>
+      </c>
+      <c r="H33" t="s">
+        <v>69</v>
+      </c>
+      <c r="I33">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G34" s="18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
+        <v>60</v>
+      </c>
+      <c r="H35" t="s">
+        <v>74</v>
+      </c>
+      <c r="I35">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="36" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>61</v>
+      </c>
+      <c r="H36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I36">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="37" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>62</v>
+      </c>
+      <c r="H37" t="s">
+        <v>74</v>
+      </c>
+      <c r="I37">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="38" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>63</v>
+      </c>
+      <c r="H38" t="s">
+        <v>74</v>
+      </c>
+      <c r="I38">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="39" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
+        <v>64</v>
+      </c>
+      <c r="H39" t="s">
+        <v>69</v>
+      </c>
+      <c r="I39">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="40" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G40" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>66</v>
+      </c>
+      <c r="H41" t="s">
+        <v>70</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
+        <v>67</v>
+      </c>
+      <c r="H42" t="s">
+        <v>75</v>
+      </c>
+      <c r="I42">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="43" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
+        <v>68</v>
+      </c>
+      <c r="H43" t="s">
+        <v>70</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G45" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="I45">
+        <f>PRODUCT(I26:I43)</f>
+        <v>2.1315674647809386</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="G4:L4"/>
@@ -1607,14 +2033,6 @@
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>